<commit_message>
Removed the peudo SQL function and added a join to Geography to the system prompt
</commit_message>
<xml_diff>
--- a/web-llm-sql-csv/db_schema.xlsx
+++ b/web-llm-sql-csv/db_schema.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tommeijer/LLM_test/web-llm-sql-csv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1B301A-88BC-DA4E-ADCB-BD344E58F00F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E91890C-7C7C-3D43-8452-355AEC921B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="660" windowWidth="34560" windowHeight="20100" xr2:uid="{9D4557AC-C91B-254A-A119-4DC8F4CB9F5C}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="38400" windowHeight="21780" activeTab="1" xr2:uid="{9D4557AC-C91B-254A-A119-4DC8F4CB9F5C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="GC7_budget" sheetId="1" r:id="rId1"/>
+    <sheet name="Geography" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="818">
   <si>
     <t>Afghanistan</t>
   </si>
@@ -1868,9 +1869,6 @@
     <t>Voluntary medical male circumcision</t>
   </si>
   <si>
-    <t>cost_input</t>
-  </si>
-  <si>
     <t>Activity Based Contracts, Community Based Org. and other service providers</t>
   </si>
   <si>
@@ -2384,7 +2382,115 @@
     <t>Travel related costs (TRC)	Travel related costs (TRC)</t>
   </si>
   <si>
-    <t>cost_group</t>
+    <t>Cost Category</t>
+  </si>
+  <si>
+    <t>Cost Input</t>
+  </si>
+  <si>
+    <t>Albania</t>
+  </si>
+  <si>
+    <t>Algeria</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>Korea (Democratic Peoples Republic)</t>
+  </si>
+  <si>
+    <t>Multicountry Americas EMMIE</t>
+  </si>
+  <si>
+    <t>Multicountry Americas ORAS-CONHU</t>
+  </si>
+  <si>
+    <t>Multicountry Eastern Africa IGAD</t>
+  </si>
+  <si>
+    <t>Multicountry EECA PAS</t>
+  </si>
+  <si>
+    <t>Multicountry HIV Latin America ALEP</t>
+  </si>
+  <si>
+    <t>Multicountry HIV MENA IHAA</t>
+  </si>
+  <si>
+    <t>Multicountry MENA Key Populations</t>
+  </si>
+  <si>
+    <t>Multicountry Southern Africa E8</t>
+  </si>
+  <si>
+    <t>Multicountry Southern Africa TIMS</t>
+  </si>
+  <si>
+    <t>Multicountry Southern Africa WHC</t>
+  </si>
+  <si>
+    <t>Multicountry TB Asia TEAM</t>
+  </si>
+  <si>
+    <t>Multicountry TB Asia UNDP</t>
+  </si>
+  <si>
+    <t>Multicountry TB Asia UNOPS</t>
+  </si>
+  <si>
+    <t>Multicountry TB LAC PIH</t>
+  </si>
+  <si>
+    <t>Multicountry TB WC Africa NTP/SRL</t>
+  </si>
+  <si>
+    <t>Multicountry West Africa ALCO</t>
+  </si>
+  <si>
+    <t>Panama</t>
+  </si>
+  <si>
+    <t>Romania</t>
+  </si>
+  <si>
+    <t>Tunisia</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>[NewRegioShort]</t>
+  </si>
+  <si>
+    <t>[Geography Name]</t>
+  </si>
+  <si>
+    <t>EECA</t>
+  </si>
+  <si>
+    <t>HIA1</t>
+  </si>
+  <si>
+    <t>HIA2</t>
+  </si>
+  <si>
+    <t>LAC</t>
+  </si>
+  <si>
+    <t>MENASEA</t>
+  </si>
+  <si>
+    <t>WCA</t>
+  </si>
+  <si>
+    <t>ALE</t>
+  </si>
+  <si>
+    <t>AME</t>
+  </si>
+  <si>
+    <t>[NewDept]</t>
   </si>
 </sst>
 </file>
@@ -2757,9 +2863,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21CD33D5-EF48-784B-BC2B-B8AC7B19DDE1}">
   <dimension ref="A1:F267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
@@ -2785,10 +2889,10 @@
         <v>418</v>
       </c>
       <c r="E1" t="s">
+        <v>781</v>
+      </c>
+      <c r="F1" t="s">
         <v>782</v>
-      </c>
-      <c r="F1" t="s">
-        <v>610</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2805,10 +2909,10 @@
         <v>460</v>
       </c>
       <c r="E2" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="F2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -2825,10 +2929,10 @@
         <v>466</v>
       </c>
       <c r="E3" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="F3" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -2845,10 +2949,10 @@
         <v>470</v>
       </c>
       <c r="E4" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="F4" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2865,10 +2969,10 @@
         <v>485</v>
       </c>
       <c r="E5" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="F5" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2885,10 +2989,10 @@
         <v>496</v>
       </c>
       <c r="E6" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="F6" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -2905,10 +3009,10 @@
         <v>500</v>
       </c>
       <c r="E7" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="F7" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -2925,10 +3029,10 @@
         <v>535</v>
       </c>
       <c r="E8" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="F8" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -2945,10 +3049,10 @@
         <v>540</v>
       </c>
       <c r="E9" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="F9" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2965,10 +3069,10 @@
         <v>588</v>
       </c>
       <c r="E10" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="F10" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2985,10 +3089,10 @@
         <v>606</v>
       </c>
       <c r="E11" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="F11" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -3005,10 +3109,10 @@
         <v>427</v>
       </c>
       <c r="E12" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="F12" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3025,10 +3129,10 @@
         <v>436</v>
       </c>
       <c r="E13" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="F13" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -3045,10 +3149,10 @@
         <v>534</v>
       </c>
       <c r="E14" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="F14" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -3065,10 +3169,10 @@
         <v>437</v>
       </c>
       <c r="E15" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="F15" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -3085,10 +3189,10 @@
         <v>438</v>
       </c>
       <c r="E16" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="F16" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -3105,10 +3209,10 @@
         <v>439</v>
       </c>
       <c r="E17" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="F17" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -3125,10 +3229,10 @@
         <v>467</v>
       </c>
       <c r="E18" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="F18" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -3145,10 +3249,10 @@
         <v>468</v>
       </c>
       <c r="E19" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="F19" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -3165,10 +3269,10 @@
         <v>469</v>
       </c>
       <c r="E20" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="F20" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -3185,10 +3289,10 @@
         <v>578</v>
       </c>
       <c r="E21" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="F21" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -3205,10 +3309,10 @@
         <v>579</v>
       </c>
       <c r="E22" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="F22" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -3225,10 +3329,10 @@
         <v>580</v>
       </c>
       <c r="E23" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="F23" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -3245,10 +3349,10 @@
         <v>455</v>
       </c>
       <c r="E24" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="F24" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -3265,10 +3369,10 @@
         <v>456</v>
       </c>
       <c r="E25" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="F25" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -3285,10 +3389,10 @@
         <v>457</v>
       </c>
       <c r="E26" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F26" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -3305,10 +3409,10 @@
         <v>498</v>
       </c>
       <c r="E27" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="F27" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -3325,10 +3429,10 @@
         <v>523</v>
       </c>
       <c r="E28" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="F28" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -3345,10 +3449,10 @@
         <v>532</v>
       </c>
       <c r="E29" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="F29" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -3365,10 +3469,10 @@
         <v>550</v>
       </c>
       <c r="E30" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="F30" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -3385,10 +3489,10 @@
         <v>503</v>
       </c>
       <c r="E31" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="F31" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -3405,10 +3509,10 @@
         <v>504</v>
       </c>
       <c r="E32" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="F32" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -3425,10 +3529,10 @@
         <v>505</v>
       </c>
       <c r="E33" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="F33" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -3445,10 +3549,10 @@
         <v>506</v>
       </c>
       <c r="E34" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="F34" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -3465,10 +3569,10 @@
         <v>507</v>
       </c>
       <c r="E35" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="F35" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -3485,10 +3589,10 @@
         <v>508</v>
       </c>
       <c r="E36" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="F36" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -3505,10 +3609,10 @@
         <v>392</v>
       </c>
       <c r="E37" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="F37" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -3525,10 +3629,10 @@
         <v>443</v>
       </c>
       <c r="E38" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="F38" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -3545,10 +3649,10 @@
         <v>444</v>
       </c>
       <c r="E39" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="F39" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -3565,10 +3669,10 @@
         <v>445</v>
       </c>
       <c r="E40" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="F40" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -3585,10 +3689,10 @@
         <v>475</v>
       </c>
       <c r="E41" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="F41" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -3605,10 +3709,10 @@
         <v>476</v>
       </c>
       <c r="E42" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="F42" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -3625,10 +3729,10 @@
         <v>524</v>
       </c>
       <c r="E43" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="F43" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -3645,10 +3749,10 @@
         <v>525</v>
       </c>
       <c r="E44" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="F44" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -3665,10 +3769,10 @@
         <v>543</v>
       </c>
       <c r="E45" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="F45" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -3685,10 +3789,10 @@
         <v>581</v>
       </c>
       <c r="E46" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="F46" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -3705,10 +3809,10 @@
         <v>592</v>
       </c>
       <c r="E47" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="F47" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -3725,10 +3829,10 @@
         <v>609</v>
       </c>
       <c r="E48" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="F48" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -3745,10 +3849,10 @@
         <v>428</v>
       </c>
       <c r="E49" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="F49" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -3765,10 +3869,10 @@
         <v>446</v>
       </c>
       <c r="E50" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="F50" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -3785,10 +3889,10 @@
         <v>477</v>
       </c>
       <c r="E51" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="F51" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -3805,10 +3909,10 @@
         <v>526</v>
       </c>
       <c r="E52" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="F52" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -3825,10 +3929,10 @@
         <v>544</v>
       </c>
       <c r="E53" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="F53" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -3845,10 +3949,10 @@
         <v>582</v>
       </c>
       <c r="E54" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="F54" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -3865,10 +3969,10 @@
         <v>429</v>
       </c>
       <c r="E55" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="F55" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -3885,10 +3989,10 @@
         <v>447</v>
       </c>
       <c r="E56" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="F56" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -3905,10 +4009,10 @@
         <v>478</v>
       </c>
       <c r="E57" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="F57" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -3925,10 +4029,10 @@
         <v>527</v>
       </c>
       <c r="E58" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="F58" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -3945,10 +4049,10 @@
         <v>545</v>
       </c>
       <c r="E59" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="F59" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -3965,10 +4069,10 @@
         <v>583</v>
       </c>
       <c r="E60" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="F60" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -3985,10 +4089,10 @@
         <v>448</v>
       </c>
       <c r="E61" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="F61" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -4005,10 +4109,10 @@
         <v>472</v>
       </c>
       <c r="E62" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="F62" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -4025,10 +4129,10 @@
         <v>479</v>
       </c>
       <c r="E63" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="F63" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -4045,10 +4149,10 @@
         <v>528</v>
       </c>
       <c r="E64" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="F64" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -4065,10 +4169,10 @@
         <v>546</v>
       </c>
       <c r="E65" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="F65" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -4085,10 +4189,10 @@
         <v>584</v>
       </c>
       <c r="E66" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="F66" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -4105,10 +4209,10 @@
         <v>430</v>
       </c>
       <c r="E67" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="F67" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -4125,10 +4229,10 @@
         <v>449</v>
       </c>
       <c r="E68" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="F68" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -4145,10 +4249,10 @@
         <v>480</v>
       </c>
       <c r="E69" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="F69" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -4165,10 +4269,10 @@
         <v>514</v>
       </c>
       <c r="E70" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="F70" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -4185,7 +4289,7 @@
         <v>516</v>
       </c>
       <c r="E71" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="F71" t="s">
         <v>392</v>
@@ -4205,10 +4309,10 @@
         <v>518</v>
       </c>
       <c r="E72" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="F72" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -4225,10 +4329,10 @@
         <v>529</v>
       </c>
       <c r="E73" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="F73" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -4245,10 +4349,10 @@
         <v>547</v>
       </c>
       <c r="E74" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="F74" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -4265,10 +4369,10 @@
         <v>585</v>
       </c>
       <c r="E75" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="F75" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -4285,10 +4389,10 @@
         <v>431</v>
       </c>
       <c r="E76" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="F76" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -4305,10 +4409,10 @@
         <v>450</v>
       </c>
       <c r="E77" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="F77" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -4325,10 +4429,10 @@
         <v>481</v>
       </c>
       <c r="E78" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="F78" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -4345,10 +4449,10 @@
         <v>530</v>
       </c>
       <c r="E79" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="F79" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -4365,10 +4469,10 @@
         <v>548</v>
       </c>
       <c r="E80" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="F80" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -4385,10 +4489,10 @@
         <v>586</v>
       </c>
       <c r="E81" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="F81" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -4405,10 +4509,10 @@
         <v>432</v>
       </c>
       <c r="E82" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="F82" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -4425,10 +4529,10 @@
         <v>451</v>
       </c>
       <c r="E83" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="F83" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -4445,10 +4549,10 @@
         <v>482</v>
       </c>
       <c r="E84" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="F84" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -4465,10 +4569,10 @@
         <v>531</v>
       </c>
       <c r="E85" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="F85" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -4485,10 +4589,10 @@
         <v>549</v>
       </c>
       <c r="E86" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="F86" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -4505,10 +4609,10 @@
         <v>587</v>
       </c>
       <c r="E87" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="F87" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -6150,6 +6254,744 @@
     <row r="267" spans="2:2">
       <c r="B267" t="s">
         <v>384</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{608073B5-9C5D-BB48-A2D9-F2B0509A40BD}">
+  <dimension ref="A1:C136"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>808</v>
+      </c>
+      <c r="B1" t="s">
+        <v>807</v>
+      </c>
+      <c r="C1" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>806</v>
+      </c>
+      <c r="C2" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>783</v>
+      </c>
+      <c r="B3" t="s">
+        <v>809</v>
+      </c>
+      <c r="C3" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>784</v>
+      </c>
+      <c r="B4" t="s">
+        <v>810</v>
+      </c>
+      <c r="C4" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>811</v>
+      </c>
+      <c r="C5" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1">
+      <c r="A50" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1">
+      <c r="A51" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1">
+      <c r="A64" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1">
+      <c r="A65" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1">
+      <c r="A105" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1">
+      <c r="A106" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>